<commit_message>
Output Azure Translate Results
</commit_message>
<xml_diff>
--- a/BLEU/EN-Dictionary/GP詞彙解釋.xlsx
+++ b/BLEU/EN-Dictionary/GP詞彙解釋.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\extract_raw-data\EN-Dictionary\Training Set\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\extract_raw-data\BLEU\EN-Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CD361E-B6B9-4E85-A863-01534A12176B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10957B7F-6AE0-4948-BAD6-0F165508ADB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="4110" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="577">
   <si>
     <t>阿羅漢</t>
   </si>
@@ -1804,6 +1804,10 @@
   </si>
   <si>
     <t>ZH-TW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Azure Translation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2168,25 +2172,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B328"/>
+  <dimension ref="A1:C328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.3984375" customWidth="1"/>
     <col min="2" max="2" width="25.19921875" customWidth="1"/>
+    <col min="3" max="3" width="37.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>575</v>
       </c>
       <c r="B1" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+      <c r="C1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2194,7 +2204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2202,7 +2212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2210,7 +2220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2218,7 +2228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2226,7 +2236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2234,7 +2244,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -2242,7 +2252,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -2250,7 +2260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -2258,7 +2268,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -2266,7 +2276,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -2274,7 +2284,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2282,7 +2292,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -2290,7 +2300,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -2298,7 +2308,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>